<commit_message>
update modred feature selection for HDAC2
</commit_message>
<xml_diff>
--- a/My HDAC2/output/Số lượng top-ranking features.xlsx
+++ b/My HDAC2/output/Số lượng top-ranking features.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\MachineLearning\JupyterNotebook\Pharmacy\My HDAC2\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\MachineLearning\JupyterNotebook\Pharmacy\My HDAC2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B2B397-5B58-4A6F-92BD-B2D407FF6253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08DC646-C796-41D2-BBD4-28661372B89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -44,6 +45,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,7 +394,7 @@
   <dimension ref="A1:B216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="S182" sqref="S182"/>
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>